<commit_message>
add active column to debts and fixed assets
</commit_message>
<xml_diff>
--- a/examples/HFP_jack+jill.xlsx
+++ b/examples/HFP_jack+jill.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Retirement\MyProject\Owl\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78C095B-2637-4002-8A66-C4C993C6A2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04B6C54-74C8-48AC-B03F-7A4DC1DBFB15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28320" activeTab="2" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
   </bookViews>
   <sheets>
     <sheet name="Jack" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>year</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>commission</t>
+  </si>
+  <si>
+    <t>active</t>
   </si>
 </sst>
 </file>
@@ -484,24 +487,24 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.81640625" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -530,7 +533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>2020</v>
       </c>
@@ -545,7 +548,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2021</v>
       </c>
@@ -560,7 +563,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>2022</v>
       </c>
@@ -575,7 +578,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>2023</v>
       </c>
@@ -590,7 +593,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>2024</v>
       </c>
@@ -607,7 +610,7 @@
       </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2025</v>
       </c>
@@ -624,7 +627,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2026</v>
       </c>
@@ -641,7 +644,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2027</v>
       </c>
@@ -658,7 +661,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2028</v>
       </c>
@@ -673,7 +676,7 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2029</v>
       </c>
@@ -686,7 +689,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2030</v>
       </c>
@@ -699,7 +702,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2031</v>
       </c>
@@ -712,7 +715,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2032</v>
       </c>
@@ -725,7 +728,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2033</v>
       </c>
@@ -738,7 +741,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2034</v>
       </c>
@@ -751,7 +754,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2035</v>
       </c>
@@ -764,7 +767,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2036</v>
       </c>
@@ -777,7 +780,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2037</v>
       </c>
@@ -790,7 +793,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2038</v>
       </c>
@@ -803,7 +806,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2039</v>
       </c>
@@ -816,7 +819,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2040</v>
       </c>
@@ -829,7 +832,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2041</v>
       </c>
@@ -842,7 +845,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2042</v>
       </c>
@@ -855,7 +858,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2043</v>
       </c>
@@ -868,7 +871,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2044</v>
       </c>
@@ -881,7 +884,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2045</v>
       </c>
@@ -894,7 +897,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2046</v>
       </c>
@@ -907,7 +910,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2047</v>
       </c>
@@ -920,7 +923,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2048</v>
       </c>
@@ -933,7 +936,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2049</v>
       </c>
@@ -946,7 +949,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2050</v>
       </c>
@@ -959,7 +962,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2051</v>
       </c>
@@ -972,7 +975,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2052</v>
       </c>
@@ -985,7 +988,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2053</v>
       </c>
@@ -998,7 +1001,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2054</v>
       </c>
@@ -1011,7 +1014,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>2055</v>
       </c>
@@ -1030,20 +1033,20 @@
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1796875" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" customWidth="1"/>
+    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1072,7 +1075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>2020</v>
       </c>
@@ -1087,7 +1090,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2021</v>
       </c>
@@ -1102,7 +1105,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>2022</v>
       </c>
@@ -1117,7 +1120,7 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>2023</v>
       </c>
@@ -1132,7 +1135,7 @@
       </c>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>2024</v>
       </c>
@@ -1147,7 +1150,7 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2025</v>
       </c>
@@ -1162,7 +1165,7 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2026</v>
       </c>
@@ -1177,7 +1180,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2027</v>
       </c>
@@ -1192,7 +1195,7 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2028</v>
       </c>
@@ -1205,7 +1208,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2029</v>
       </c>
@@ -1218,7 +1221,7 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2030</v>
       </c>
@@ -1231,7 +1234,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2031</v>
       </c>
@@ -1244,7 +1247,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2032</v>
       </c>
@@ -1257,7 +1260,7 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2033</v>
       </c>
@@ -1270,7 +1273,7 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2034</v>
       </c>
@@ -1283,7 +1286,7 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2035</v>
       </c>
@@ -1296,7 +1299,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2036</v>
       </c>
@@ -1309,7 +1312,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2037</v>
       </c>
@@ -1322,7 +1325,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2038</v>
       </c>
@@ -1335,7 +1338,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2039</v>
       </c>
@@ -1348,7 +1351,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2040</v>
       </c>
@@ -1361,7 +1364,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2041</v>
       </c>
@@ -1374,7 +1377,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2042</v>
       </c>
@@ -1387,7 +1390,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2043</v>
       </c>
@@ -1400,7 +1403,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2044</v>
       </c>
@@ -1413,7 +1416,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2045</v>
       </c>
@@ -1426,7 +1429,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2046</v>
       </c>
@@ -1439,7 +1442,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2047</v>
       </c>
@@ -1452,7 +1455,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2048</v>
       </c>
@@ -1465,7 +1468,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2049</v>
       </c>
@@ -1478,7 +1481,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2050</v>
       </c>
@@ -1491,7 +1494,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2051</v>
       </c>
@@ -1504,7 +1507,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2052</v>
       </c>
@@ -1517,7 +1520,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2053</v>
       </c>
@@ -1530,7 +1533,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2054</v>
       </c>
@@ -1543,7 +1546,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>2055</v>
       </c>
@@ -1556,7 +1559,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>2056</v>
       </c>
@@ -1569,12 +1572,12 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>2057</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>2058</v>
       </c>
@@ -1586,40 +1589,43 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA707BF-A4A7-4841-BFD6-9B94FB900DD0}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="10.28515625" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" customWidth="1"/>
+    <col min="1" max="2" width="12.26953125" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" customWidth="1"/>
+    <col min="4" max="4" width="8.453125" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" style="1"/>
+    <col min="7" max="7" width="10.26953125" customWidth="1"/>
+    <col min="12" max="12" width="11.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1630,41 +1636,44 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29335860-5C91-4189-B35F-4DDEB06D1DBA}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.26953125" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
year shifted all cases
</commit_message>
<xml_diff>
--- a/examples/HFP_jack+jill.xlsx
+++ b/examples/HFP_jack+jill.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Retirement\MyProject\Owl\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04B6C54-74C8-48AC-B03F-7A4DC1DBFB15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FD92FA-2D47-490F-BE2A-440C9A9818E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
   </bookViews>
   <sheets>
     <sheet name="Jack" sheetId="1" r:id="rId1"/>
@@ -481,10 +481,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB57614-FCF1-4139-AA0D-31AF55A08D66}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A2" sqref="A2:A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -535,7 +535,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -550,7 +550,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -565,7 +565,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -580,7 +580,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -594,8 +594,8 @@
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
-        <v>2024</v>
+      <c r="A6">
+        <v>2025</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -612,7 +612,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B7" s="1">
         <v>100000</v>
@@ -629,7 +629,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="B8" s="1">
         <v>100000</v>
@@ -646,7 +646,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="B9" s="1">
         <v>100000</v>
@@ -663,7 +663,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -678,7 +678,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -691,7 +691,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -704,7 +704,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -717,7 +717,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -730,7 +730,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -743,7 +743,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>2034</v>
+        <v>2035</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -756,7 +756,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -769,7 +769,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -782,7 +782,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -795,7 +795,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -808,7 +808,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -821,7 +821,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -834,7 +834,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -847,7 +847,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -860,7 +860,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -873,7 +873,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>2044</v>
+        <v>2045</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -886,7 +886,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -899,7 +899,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -912,7 +912,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>2047</v>
+        <v>2048</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -925,7 +925,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>2048</v>
+        <v>2049</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -938,7 +938,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>2049</v>
+        <v>2050</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -951,7 +951,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>2050</v>
+        <v>2051</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -964,7 +964,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>2051</v>
+        <v>2052</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -977,7 +977,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>2052</v>
+        <v>2053</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -990,7 +990,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35">
-        <v>2053</v>
+        <v>2054</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1003,7 +1003,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36">
-        <v>2054</v>
+        <v>2055</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1014,11 +1014,6 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37">
-        <v>2055</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1027,10 +1022,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DE7EE4-731B-47FB-9A4E-667972814602}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1077,7 +1072,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1092,7 +1087,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1107,7 +1102,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1122,7 +1117,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1136,8 +1131,8 @@
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
-        <v>2024</v>
+      <c r="A6">
+        <v>2025</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1152,7 +1147,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="B7" s="6">
         <v>80000</v>
@@ -1167,7 +1162,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="B8" s="6">
         <v>80000</v>
@@ -1182,7 +1177,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="B9" s="6">
         <v>85000</v>
@@ -1197,7 +1192,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1210,7 +1205,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1223,7 +1218,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1236,7 +1231,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1249,7 +1244,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1262,7 +1257,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1275,7 +1270,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>2034</v>
+        <v>2035</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1288,7 +1283,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1301,7 +1296,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1314,7 +1309,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1327,7 +1322,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1340,7 +1335,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1353,7 +1348,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1366,7 +1361,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1379,7 +1374,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1392,7 +1387,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1405,7 +1400,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>2044</v>
+        <v>2045</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1418,7 +1413,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1431,7 +1426,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1444,7 +1439,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>2047</v>
+        <v>2048</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1457,7 +1452,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>2048</v>
+        <v>2049</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1470,7 +1465,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>2049</v>
+        <v>2050</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1483,7 +1478,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>2050</v>
+        <v>2051</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1496,7 +1491,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>2051</v>
+        <v>2052</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1509,7 +1504,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>2052</v>
+        <v>2053</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1522,7 +1517,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35">
-        <v>2053</v>
+        <v>2054</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1535,7 +1530,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36">
-        <v>2054</v>
+        <v>2055</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1548,7 +1543,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>2055</v>
+        <v>2056</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1561,7 +1556,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38">
-        <v>2056</v>
+        <v>2057</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1574,11 +1569,6 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39">
-        <v>2057</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40">
         <v>2058</v>
       </c>
     </row>
@@ -1638,7 +1628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29335860-5C91-4189-B35F-4DDEB06D1DBA}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add year for Fixed Assets issue#57
</commit_message>
<xml_diff>
--- a/examples/HFP_jack+jill.xlsx
+++ b/examples/HFP_jack+jill.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Retirement\MyProject\Owl\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdlacasse/Owl/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FD92FA-2D47-490F-BE2A-440C9A9818E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD35A25-49E6-9B4A-A20A-9670F53C2694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
   </bookViews>
   <sheets>
     <sheet name="Jack" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>year</t>
   </si>
@@ -487,24 +487,24 @@
       <selection activeCell="A2" sqref="A2:A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.81640625" customWidth="1"/>
-    <col min="2" max="2" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -533,7 +533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>2021</v>
       </c>
@@ -548,7 +548,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2022</v>
       </c>
@@ -563,7 +563,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2023</v>
       </c>
@@ -578,7 +578,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2024</v>
       </c>
@@ -593,7 +593,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2025</v>
       </c>
@@ -610,7 +610,7 @@
       </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2026</v>
       </c>
@@ -627,7 +627,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2027</v>
       </c>
@@ -644,7 +644,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2028</v>
       </c>
@@ -661,7 +661,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2029</v>
       </c>
@@ -676,7 +676,7 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2030</v>
       </c>
@@ -689,7 +689,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2031</v>
       </c>
@@ -702,7 +702,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2032</v>
       </c>
@@ -715,7 +715,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2033</v>
       </c>
@@ -728,7 +728,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2034</v>
       </c>
@@ -741,7 +741,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2035</v>
       </c>
@@ -754,7 +754,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2036</v>
       </c>
@@ -767,7 +767,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2037</v>
       </c>
@@ -780,7 +780,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2038</v>
       </c>
@@ -793,7 +793,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2039</v>
       </c>
@@ -806,7 +806,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2040</v>
       </c>
@@ -819,7 +819,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2041</v>
       </c>
@@ -832,7 +832,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2042</v>
       </c>
@@ -845,7 +845,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2043</v>
       </c>
@@ -858,7 +858,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2044</v>
       </c>
@@ -871,7 +871,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2045</v>
       </c>
@@ -884,7 +884,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2046</v>
       </c>
@@ -897,7 +897,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2047</v>
       </c>
@@ -910,7 +910,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2048</v>
       </c>
@@ -923,7 +923,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2049</v>
       </c>
@@ -936,7 +936,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2050</v>
       </c>
@@ -949,7 +949,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2051</v>
       </c>
@@ -962,7 +962,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2052</v>
       </c>
@@ -975,7 +975,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2053</v>
       </c>
@@ -988,7 +988,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2054</v>
       </c>
@@ -1001,7 +1001,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2055</v>
       </c>
@@ -1024,24 +1024,24 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" customWidth="1"/>
-    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" customWidth="1"/>
-    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>2021</v>
       </c>
@@ -1085,7 +1085,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2022</v>
       </c>
@@ -1100,7 +1100,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2023</v>
       </c>
@@ -1115,7 +1115,7 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2024</v>
       </c>
@@ -1130,7 +1130,7 @@
       </c>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2025</v>
       </c>
@@ -1145,7 +1145,7 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2026</v>
       </c>
@@ -1160,7 +1160,7 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2027</v>
       </c>
@@ -1175,7 +1175,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2028</v>
       </c>
@@ -1190,7 +1190,7 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2029</v>
       </c>
@@ -1203,7 +1203,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2030</v>
       </c>
@@ -1216,7 +1216,7 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2031</v>
       </c>
@@ -1229,7 +1229,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2032</v>
       </c>
@@ -1242,7 +1242,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2033</v>
       </c>
@@ -1255,7 +1255,7 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2034</v>
       </c>
@@ -1268,7 +1268,7 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2035</v>
       </c>
@@ -1281,7 +1281,7 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2036</v>
       </c>
@@ -1294,7 +1294,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2037</v>
       </c>
@@ -1307,7 +1307,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2038</v>
       </c>
@@ -1320,7 +1320,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2039</v>
       </c>
@@ -1333,7 +1333,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2040</v>
       </c>
@@ -1346,7 +1346,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2041</v>
       </c>
@@ -1359,7 +1359,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2042</v>
       </c>
@@ -1372,7 +1372,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2043</v>
       </c>
@@ -1385,7 +1385,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2044</v>
       </c>
@@ -1398,7 +1398,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2045</v>
       </c>
@@ -1411,7 +1411,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2046</v>
       </c>
@@ -1424,7 +1424,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2047</v>
       </c>
@@ -1437,7 +1437,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2048</v>
       </c>
@@ -1450,7 +1450,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2049</v>
       </c>
@@ -1463,7 +1463,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2050</v>
       </c>
@@ -1476,7 +1476,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2051</v>
       </c>
@@ -1489,7 +1489,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2052</v>
       </c>
@@ -1502,7 +1502,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2053</v>
       </c>
@@ -1515,7 +1515,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2054</v>
       </c>
@@ -1528,7 +1528,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2055</v>
       </c>
@@ -1541,7 +1541,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2056</v>
       </c>
@@ -1554,7 +1554,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2057</v>
       </c>
@@ -1567,7 +1567,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2058</v>
       </c>
@@ -1582,21 +1582,21 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="12.26953125" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" customWidth="1"/>
-    <col min="4" max="4" width="8.453125" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" style="1"/>
-    <col min="7" max="7" width="10.26953125" customWidth="1"/>
-    <col min="12" max="12" width="11.81640625" customWidth="1"/>
+    <col min="1" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
+    <col min="4" max="4" width="8.5" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" style="1"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
@@ -1626,22 +1626,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29335860-5C91-4189-B35F-4DDEB06D1DBA}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.26953125" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1796875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.26953125" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
@@ -1651,19 +1652,22 @@
       <c r="C1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>